<commit_message>
Added option to allow inserting default values for columns that are NOT NULL
</commit_message>
<xml_diff>
--- a/testdata/load.xlsx
+++ b/testdata/load.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED280EF-1C1A-4A0E-A27B-CBEA15767006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17D8334-CA74-4AC4-8476-7D8641C9DADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-10910" windowWidth="38620" windowHeight="21360" tabRatio="825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="会社" sheetId="89" r:id="rId1"/>
+    <sheet name="normal-テストx" sheetId="89" r:id="rId1"/>
+    <sheet name="option-テストx" sheetId="90" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="78">
   <si>
     <t>項目物理名</t>
     <rPh sb="0" eb="2">
@@ -78,30 +79,10 @@
     <phoneticPr fontId="12"/>
   </si>
   <si>
-    <t>更新日時</t>
-  </si>
-  <si>
     <t>開始</t>
   </si>
   <si>
-    <t>N</t>
-    <phoneticPr fontId="12"/>
-  </si>
-  <si>
     <t>C</t>
-    <phoneticPr fontId="12"/>
-  </si>
-  <si>
-    <t>created_at</t>
-  </si>
-  <si>
-    <t>updated_at</t>
-  </si>
-  <si>
-    <t>作成日時</t>
-  </si>
-  <si>
-    <t>current_timestamp</t>
     <phoneticPr fontId="12"/>
   </si>
   <si>
@@ -118,93 +99,227 @@
     <t>timestamp with time zone</t>
   </si>
   <si>
-    <t>revision</t>
+    <t>id</t>
   </si>
   <si>
-    <t>sys</t>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>bytea</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>real</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>double precision</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>json</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>jsonb</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>inet</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>smallint</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>bigint</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>interval</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>oid</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>time without time zone</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>timestamp without time zone</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>uuid</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>true</t>
     <phoneticPr fontId="12"/>
   </si>
   <si>
-    <t>終了</t>
-    <rPh sb="0" eb="2">
-      <t>シュウリョウ</t>
-    </rPh>
+    <t>bytea</t>
     <phoneticPr fontId="12"/>
   </si>
   <si>
-    <t>会社</t>
-    <rPh sb="0" eb="2">
-      <t>カイシャ</t>
-    </rPh>
+    <t>a</t>
     <phoneticPr fontId="12"/>
   </si>
   <si>
-    <t>company</t>
+    <t>2022-01-01</t>
     <phoneticPr fontId="12"/>
   </si>
   <si>
-    <t>創業年</t>
-    <rPh sb="0" eb="3">
-      <t>ソウギョウネン</t>
-    </rPh>
+    <t>0.1</t>
     <phoneticPr fontId="12"/>
   </si>
   <si>
-    <t>founded_year</t>
+    <t>0.01</t>
     <phoneticPr fontId="12"/>
   </si>
   <si>
-    <t>会社コード</t>
+    <t>{}</t>
     <phoneticPr fontId="12"/>
   </si>
   <si>
-    <t>リビジョン</t>
-    <phoneticPr fontId="12"/>
-  </si>
-  <si>
-    <t>00002</t>
-    <phoneticPr fontId="12"/>
-  </si>
-  <si>
-    <t>1989</t>
-    <phoneticPr fontId="12"/>
-  </si>
-  <si>
-    <t>1972</t>
-    <phoneticPr fontId="12"/>
-  </si>
-  <si>
-    <t>会社名</t>
-    <rPh sb="0" eb="2">
-      <t>カイシャ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>メイ</t>
-    </rPh>
-    <phoneticPr fontId="12"/>
-  </si>
-  <si>
-    <t>company_cd</t>
-    <phoneticPr fontId="12"/>
-  </si>
-  <si>
-    <t>company_name</t>
-    <phoneticPr fontId="12"/>
-  </si>
-  <si>
-    <t>00001</t>
-    <phoneticPr fontId="12"/>
-  </si>
-  <si>
-    <t>Future</t>
-    <phoneticPr fontId="12"/>
-  </si>
-  <si>
-    <t>YDC</t>
+    <t>0.0.0.0</t>
     <phoneticPr fontId="12"/>
   </si>
   <si>
     <t>1</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>32767</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>2147483647</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>9223372036854775807</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>11111</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>test</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>01:02:03</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>2022-01-01 01:02:03</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>2022-01-01 01:02:03+09</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>cee0db76-d69c-4ae3-ae33-5b5970adde48</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>abc</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>test1</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>test_x</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>テストx</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>test-opt</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>z</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>bit</t>
     <phoneticPr fontId="12"/>
   </si>
 </sst>
@@ -14592,133 +14707,7 @@
     <cellStyle name="湪＀〰〰ヿ〰〰丰" xfId="5871" xr:uid="{00000000-0005-0000-0000-0000E9180000}"/>
     <cellStyle name="㼿㼿㼿㼿㼿㼿㼿" xfId="5872" xr:uid="{00000000-0005-0000-0000-0000EA180000}"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -15167,7 +15156,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F818B3D-F701-434C-A255-6A91A94F7231}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -15180,84 +15169,117 @@
     <col min="5" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:24">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="4" spans="1:7" s="11" customFormat="1">
+    <row r="4" spans="1:24" s="11" customFormat="1">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
-      <c r="E4" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>19</v>
-      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
     </row>
-    <row r="5" spans="1:7" s="6" customFormat="1">
+    <row r="5" spans="1:24" s="6" customFormat="1">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
-      <c r="G5" s="12" t="s">
-        <v>20</v>
-      </c>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
     </row>
-    <row r="6" spans="1:7" s="6" customFormat="1">
+    <row r="6" spans="1:24" s="6" customFormat="1">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>8</v>
-      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
     </row>
-    <row r="7" spans="1:7" s="9" customFormat="1">
+    <row r="7" spans="1:24" s="9" customFormat="1">
       <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>15</v>
@@ -15266,200 +15288,397 @@
         <v>17</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N7" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q7" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="R7" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="S7" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="T7" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="U7" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="V7" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="W7" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="X7" s="16" t="s">
+        <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="9" customFormat="1">
+    <row r="8" spans="1:24" s="9" customFormat="1">
       <c r="A8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>25</v>
+      <c r="B8" s="14" t="s">
+        <v>12</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>23</v>
+      <c r="L8" s="14" t="s">
+        <v>32</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>12</v>
+      <c r="M8" s="14" t="s">
+        <v>33</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>6</v>
+      <c r="N8" s="14" t="s">
+        <v>35</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>26</v>
+      <c r="O8" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="P8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q8" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="R8" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="S8" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="T8" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="U8" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="V8" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="W8" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="X8" s="14" t="s">
+        <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="9" customFormat="1">
+    <row r="9" spans="1:24" s="9" customFormat="1">
       <c r="A9" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="C9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>24</v>
+      <c r="M9" s="14" t="s">
+        <v>33</v>
       </c>
-      <c r="E9" s="14" t="s">
-        <v>10</v>
+      <c r="N9" s="14" t="s">
+        <v>35</v>
       </c>
-      <c r="F9" s="14" t="s">
-        <v>11</v>
+      <c r="O9" s="14" t="s">
+        <v>37</v>
       </c>
-      <c r="G9" s="14" t="s">
-        <v>18</v>
+      <c r="P9" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q9" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="R9" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="S9" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="T9" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="U9" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="V9" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="W9" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="X9" s="14" t="s">
+        <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:24">
       <c r="A10" s="17">
         <v>1</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="17">
-        <v>2</v>
+      <c r="H10" s="15" t="s">
+        <v>57</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>27</v>
+      <c r="I10" s="15" t="s">
+        <v>58</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>35</v>
+      <c r="J10" s="15" t="s">
+        <v>58</v>
       </c>
-      <c r="D11" s="15" t="s">
-        <v>29</v>
+      <c r="K10" s="15" t="s">
+        <v>59</v>
       </c>
-      <c r="E11" s="15" t="s">
-        <v>13</v>
+      <c r="L10" s="15" t="s">
+        <v>61</v>
       </c>
-      <c r="F11" s="15" t="s">
-        <v>13</v>
+      <c r="M10" s="15" t="s">
+        <v>62</v>
       </c>
-      <c r="G11" s="15" t="s">
-        <v>14</v>
+      <c r="N10" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="O10" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="P10" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q10" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="R10" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="S10" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="T10" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="U10" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="V10" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="W10" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="X10" s="15" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="12"/>
-  <conditionalFormatting sqref="B5:D5 E5:G9 B8:C9">
-    <cfRule type="expression" dxfId="23" priority="143">
+  <conditionalFormatting sqref="B5:W9">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>B$4="SYS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="144">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>B$4&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:C6">
-    <cfRule type="expression" dxfId="21" priority="141">
+  <conditionalFormatting sqref="X5:X9">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>X$4="SYS"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>X$4&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40883182-E9BA-4629-B6EC-E4CFA84548FC}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
+  <cols>
+    <col min="1" max="1" width="10.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.625" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="4" spans="1:2" s="11" customFormat="1">
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="6" customFormat="1">
+      <c r="A5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="6" customFormat="1">
+      <c r="A6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="9" customFormat="1">
+      <c r="A7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="9" customFormat="1">
+      <c r="A8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="8"/>
+    </row>
+    <row r="9" spans="1:2" s="9" customFormat="1">
+      <c r="A9" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="17">
+        <v>1</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="12"/>
+  <conditionalFormatting sqref="B5:B9">
+    <cfRule type="expression" dxfId="3" priority="23">
       <formula>B$4="SYS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="142">
+    <cfRule type="expression" dxfId="2" priority="24">
       <formula>B$4&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8:C9">
-    <cfRule type="expression" dxfId="19" priority="139">
-      <formula>C$4="SYS"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="140">
-      <formula>C$4&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="17" priority="137">
-      <formula>C$4="SYS"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="138">
-      <formula>C$4&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7:C7">
-    <cfRule type="expression" dxfId="15" priority="55">
-      <formula>B$4="SYS"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="56">
-      <formula>B$4&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="13" priority="53">
-      <formula>C$4="SYS"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="54">
-      <formula>C$4&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D9">
-    <cfRule type="expression" dxfId="11" priority="11">
-      <formula>D$4="SYS"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12">
-      <formula>D$4&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="9" priority="9">
-      <formula>D$4="SYS"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="10">
-      <formula>D$4&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D9">
-    <cfRule type="expression" dxfId="7" priority="7">
-      <formula>D$4="SYS"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8">
-      <formula>D$4&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="5" priority="5">
-      <formula>D$4="SYS"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
-      <formula>D$4&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>D$4="SYS"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>D$4&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>D$4="SYS"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
-      <formula>D$4&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added option to allow inserting default values for columns that are NOT NULL (#25)
* Added option to allow inserting default values for columns that are NOT NULL

* fix review
</commit_message>
<xml_diff>
--- a/testdata/load.xlsx
+++ b/testdata/load.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED280EF-1C1A-4A0E-A27B-CBEA15767006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17D8334-CA74-4AC4-8476-7D8641C9DADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-10910" windowWidth="38620" windowHeight="21360" tabRatio="825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="会社" sheetId="89" r:id="rId1"/>
+    <sheet name="normal-テストx" sheetId="89" r:id="rId1"/>
+    <sheet name="option-テストx" sheetId="90" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="78">
   <si>
     <t>項目物理名</t>
     <rPh sb="0" eb="2">
@@ -78,30 +79,10 @@
     <phoneticPr fontId="12"/>
   </si>
   <si>
-    <t>更新日時</t>
-  </si>
-  <si>
     <t>開始</t>
   </si>
   <si>
-    <t>N</t>
-    <phoneticPr fontId="12"/>
-  </si>
-  <si>
     <t>C</t>
-    <phoneticPr fontId="12"/>
-  </si>
-  <si>
-    <t>created_at</t>
-  </si>
-  <si>
-    <t>updated_at</t>
-  </si>
-  <si>
-    <t>作成日時</t>
-  </si>
-  <si>
-    <t>current_timestamp</t>
     <phoneticPr fontId="12"/>
   </si>
   <si>
@@ -118,93 +99,227 @@
     <t>timestamp with time zone</t>
   </si>
   <si>
-    <t>revision</t>
+    <t>id</t>
   </si>
   <si>
-    <t>sys</t>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>bytea</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>real</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>double precision</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>json</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>jsonb</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>inet</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>smallint</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>bigint</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>interval</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>oid</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>time without time zone</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>timestamp without time zone</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>uuid</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>true</t>
     <phoneticPr fontId="12"/>
   </si>
   <si>
-    <t>終了</t>
-    <rPh sb="0" eb="2">
-      <t>シュウリョウ</t>
-    </rPh>
+    <t>bytea</t>
     <phoneticPr fontId="12"/>
   </si>
   <si>
-    <t>会社</t>
-    <rPh sb="0" eb="2">
-      <t>カイシャ</t>
-    </rPh>
+    <t>a</t>
     <phoneticPr fontId="12"/>
   </si>
   <si>
-    <t>company</t>
+    <t>2022-01-01</t>
     <phoneticPr fontId="12"/>
   </si>
   <si>
-    <t>創業年</t>
-    <rPh sb="0" eb="3">
-      <t>ソウギョウネン</t>
-    </rPh>
+    <t>0.1</t>
     <phoneticPr fontId="12"/>
   </si>
   <si>
-    <t>founded_year</t>
+    <t>0.01</t>
     <phoneticPr fontId="12"/>
   </si>
   <si>
-    <t>会社コード</t>
+    <t>{}</t>
     <phoneticPr fontId="12"/>
   </si>
   <si>
-    <t>リビジョン</t>
-    <phoneticPr fontId="12"/>
-  </si>
-  <si>
-    <t>00002</t>
-    <phoneticPr fontId="12"/>
-  </si>
-  <si>
-    <t>1989</t>
-    <phoneticPr fontId="12"/>
-  </si>
-  <si>
-    <t>1972</t>
-    <phoneticPr fontId="12"/>
-  </si>
-  <si>
-    <t>会社名</t>
-    <rPh sb="0" eb="2">
-      <t>カイシャ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>メイ</t>
-    </rPh>
-    <phoneticPr fontId="12"/>
-  </si>
-  <si>
-    <t>company_cd</t>
-    <phoneticPr fontId="12"/>
-  </si>
-  <si>
-    <t>company_name</t>
-    <phoneticPr fontId="12"/>
-  </si>
-  <si>
-    <t>00001</t>
-    <phoneticPr fontId="12"/>
-  </si>
-  <si>
-    <t>Future</t>
-    <phoneticPr fontId="12"/>
-  </si>
-  <si>
-    <t>YDC</t>
+    <t>0.0.0.0</t>
     <phoneticPr fontId="12"/>
   </si>
   <si>
     <t>1</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>32767</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>2147483647</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>9223372036854775807</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>11111</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>test</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>01:02:03</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>2022-01-01 01:02:03</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>2022-01-01 01:02:03+09</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>cee0db76-d69c-4ae3-ae33-5b5970adde48</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>abc</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>test1</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>test_x</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>テストx</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>test-opt</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>z</t>
+    <phoneticPr fontId="12"/>
+  </si>
+  <si>
+    <t>bit</t>
     <phoneticPr fontId="12"/>
   </si>
 </sst>
@@ -14592,133 +14707,7 @@
     <cellStyle name="湪＀〰〰ヿ〰〰丰" xfId="5871" xr:uid="{00000000-0005-0000-0000-0000E9180000}"/>
     <cellStyle name="㼿㼿㼿㼿㼿㼿㼿" xfId="5872" xr:uid="{00000000-0005-0000-0000-0000EA180000}"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -15167,7 +15156,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F818B3D-F701-434C-A255-6A91A94F7231}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -15180,84 +15169,117 @@
     <col min="5" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:24">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="4" spans="1:7" s="11" customFormat="1">
+    <row r="4" spans="1:24" s="11" customFormat="1">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
-      <c r="E4" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>19</v>
-      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
     </row>
-    <row r="5" spans="1:7" s="6" customFormat="1">
+    <row r="5" spans="1:24" s="6" customFormat="1">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
-      <c r="G5" s="12" t="s">
-        <v>20</v>
-      </c>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
     </row>
-    <row r="6" spans="1:7" s="6" customFormat="1">
+    <row r="6" spans="1:24" s="6" customFormat="1">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>8</v>
-      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
     </row>
-    <row r="7" spans="1:7" s="9" customFormat="1">
+    <row r="7" spans="1:24" s="9" customFormat="1">
       <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>15</v>
@@ -15266,200 +15288,397 @@
         <v>17</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N7" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q7" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="R7" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="S7" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="T7" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="U7" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="V7" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="W7" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="X7" s="16" t="s">
+        <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="9" customFormat="1">
+    <row r="8" spans="1:24" s="9" customFormat="1">
       <c r="A8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>25</v>
+      <c r="B8" s="14" t="s">
+        <v>12</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>23</v>
+      <c r="L8" s="14" t="s">
+        <v>32</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>12</v>
+      <c r="M8" s="14" t="s">
+        <v>33</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>6</v>
+      <c r="N8" s="14" t="s">
+        <v>35</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>26</v>
+      <c r="O8" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="P8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q8" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="R8" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="S8" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="T8" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="U8" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="V8" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="W8" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="X8" s="14" t="s">
+        <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="9" customFormat="1">
+    <row r="9" spans="1:24" s="9" customFormat="1">
       <c r="A9" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="C9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>24</v>
+      <c r="M9" s="14" t="s">
+        <v>33</v>
       </c>
-      <c r="E9" s="14" t="s">
-        <v>10</v>
+      <c r="N9" s="14" t="s">
+        <v>35</v>
       </c>
-      <c r="F9" s="14" t="s">
-        <v>11</v>
+      <c r="O9" s="14" t="s">
+        <v>37</v>
       </c>
-      <c r="G9" s="14" t="s">
-        <v>18</v>
+      <c r="P9" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q9" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="R9" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="S9" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="T9" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="U9" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="V9" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="W9" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="X9" s="14" t="s">
+        <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:24">
       <c r="A10" s="17">
         <v>1</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="17">
-        <v>2</v>
+      <c r="H10" s="15" t="s">
+        <v>57</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>27</v>
+      <c r="I10" s="15" t="s">
+        <v>58</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>35</v>
+      <c r="J10" s="15" t="s">
+        <v>58</v>
       </c>
-      <c r="D11" s="15" t="s">
-        <v>29</v>
+      <c r="K10" s="15" t="s">
+        <v>59</v>
       </c>
-      <c r="E11" s="15" t="s">
-        <v>13</v>
+      <c r="L10" s="15" t="s">
+        <v>61</v>
       </c>
-      <c r="F11" s="15" t="s">
-        <v>13</v>
+      <c r="M10" s="15" t="s">
+        <v>62</v>
       </c>
-      <c r="G11" s="15" t="s">
-        <v>14</v>
+      <c r="N10" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="O10" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="P10" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q10" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="R10" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="S10" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="T10" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="U10" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="V10" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="W10" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="X10" s="15" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="12"/>
-  <conditionalFormatting sqref="B5:D5 E5:G9 B8:C9">
-    <cfRule type="expression" dxfId="23" priority="143">
+  <conditionalFormatting sqref="B5:W9">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>B$4="SYS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="144">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>B$4&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:C6">
-    <cfRule type="expression" dxfId="21" priority="141">
+  <conditionalFormatting sqref="X5:X9">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>X$4="SYS"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>X$4&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40883182-E9BA-4629-B6EC-E4CFA84548FC}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
+  <cols>
+    <col min="1" max="1" width="10.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.625" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="4" spans="1:2" s="11" customFormat="1">
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="6" customFormat="1">
+      <c r="A5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="6" customFormat="1">
+      <c r="A6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="9" customFormat="1">
+      <c r="A7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="9" customFormat="1">
+      <c r="A8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="8"/>
+    </row>
+    <row r="9" spans="1:2" s="9" customFormat="1">
+      <c r="A9" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="17">
+        <v>1</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="12"/>
+  <conditionalFormatting sqref="B5:B9">
+    <cfRule type="expression" dxfId="3" priority="23">
       <formula>B$4="SYS"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="142">
+    <cfRule type="expression" dxfId="2" priority="24">
       <formula>B$4&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8:C9">
-    <cfRule type="expression" dxfId="19" priority="139">
-      <formula>C$4="SYS"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="140">
-      <formula>C$4&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="17" priority="137">
-      <formula>C$4="SYS"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="138">
-      <formula>C$4&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7:C7">
-    <cfRule type="expression" dxfId="15" priority="55">
-      <formula>B$4="SYS"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="56">
-      <formula>B$4&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="13" priority="53">
-      <formula>C$4="SYS"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="54">
-      <formula>C$4&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D9">
-    <cfRule type="expression" dxfId="11" priority="11">
-      <formula>D$4="SYS"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12">
-      <formula>D$4&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="9" priority="9">
-      <formula>D$4="SYS"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="10">
-      <formula>D$4&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D9">
-    <cfRule type="expression" dxfId="7" priority="7">
-      <formula>D$4="SYS"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8">
-      <formula>D$4&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="5" priority="5">
-      <formula>D$4="SYS"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
-      <formula>D$4&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>D$4="SYS"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>D$4&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>D$4="SYS"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
-      <formula>D$4&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>